<commit_message>
updated validateTicketMapping.xaml. Removed the unnecessary listOfUniqueDaysVariable, ensured the new_config and configExcel files are being used. And added append range statements for business exceptions. There is an odd issue where it appears the first business exception is added twice if there is more than one business exception being added.
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E787035-C177-4C29-B1C3-7D16D7BA7A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A876A-CC0A-4E4A-AAFC-5F2F09EA8077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7935" yWindow="2865" windowWidth="35580" windowHeight="15855" activeTab="1" xr2:uid="{F2E7DB86-A902-49A5-8FFE-3B34A02633B7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F2E7DB86-A902-49A5-8FFE-3B34A02633B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Business Exceptions" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,9 +386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACD85E5-474C-4ECE-9285-6A9AC8799785}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -394,9 +398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493BFA02-E12E-4E44-8728-15277AFB2D31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed the duplication issue mentioned in the previous commit.
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S\Documents\UiPath_2\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426A876A-CC0A-4E4A-AAFC-5F2F09EA8077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82097CA1-F483-4572-8122-C2DD66EA7584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F2E7DB86-A902-49A5-8FFE-3B34A02633B7}"/>
   </bookViews>
@@ -386,7 +386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACD85E5-474C-4ECE-9285-6A9AC8799785}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>

<commit_message>
finally able to convert output Excel file to PDF
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -538,6 +538,46 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
+    <x:row r="31" spans="1:1">
+      <x:c r="A31" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:1">
+      <x:c r="A32" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:1">
+      <x:c r="A33" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:1">
+      <x:c r="A34" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:1">
+      <x:c r="A35" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:1">
+      <x:c r="A36" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:1">
+      <x:c r="A37" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:1">
+      <x:c r="A38" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
was able to convert Exceptions.xlsx and outputExcel.xlsx to PDF
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <x:si>
     <x:t>The Conclusion Evidence Location path: \\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf for the change: CHANGES - SOX Audit Report for testqcl12.txt_07.01.73.eml made on 1/24/2020 is not a valid path.</x:t>
   </x:si>
   <x:si>
     <x:t>The Conclusion Evidence Location path: \\MainFolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf for the change: CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73.eml made on 1/22/2020 is not a valid path.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Conclusion Evidence Location path: \\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf for the change: CHANGES - SOX Audit Report for testps9023.txt_07.01.73.eml made on 1/9/2020 is not a valid path.</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -400,6 +403,22 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="A4" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="A5" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="A6" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:8"/>
     <x:row r="18" spans="1:8"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
ValidateEmailsWithChanges will now catch business exceptions
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -1,46 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3C1EFCF250D5557E188AE2BD49FACF9A525086BA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E5ABEC3B-1415-44C5-8D97-52967C31A3D0}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Business Exceptions" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <x:si>
-    <x:t>The Conclusion Evidence Location path: \\MainFolder\Remediation_or_Justification Evidence\1-24-2020\CHR0000382957.pdf for the change: CHANGES - SOX Audit Report for testqcl12.txt_07.01.73.eml made on 1/24/2020 is not a valid path.</x:t>
-  </x:si>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <x:si>
     <x:t>The Conclusion Evidence Location path: \\MainFolder\Remediation_or_Justification Evidence\1-22-2020\CHR0000391114.pdf for the change: CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73.eml made on 1/22/2020 is not a valid path.</x:t>
   </x:si>
-  <x:si>
-    <x:t>The Conclusion Evidence Location path: \\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf for the change: CHANGES - SOX Audit Report for testps9023.txt_07.01.73.eml made on 1/9/2020 is not a valid path.</x:t>
-  </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
+  <x:fonts count="1">
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -56,22 +44,30 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -80,19 +76,10 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -375,51 +362,22 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:A1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="H18" sqref="H18 H18:H18 A1:XFD1048576"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:8">
-      <x:c r="A1" s="1" t="s">
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:8">
-      <x:c r="A2" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:8">
-      <x:c r="A5" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:8">
-      <x:c r="A6" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:8"/>
-    <x:row r="18" spans="1:8"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
added excel formatting to workflow 5
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -1,112 +1,92 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{30DBA732-B49A-4B94-9AE0-86637A810B19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22B8DFFB-ABA0-4DAA-B7FA-9CA659D0E1D7}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="4356" yWindow="2604" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{E61F36DB-E3C1-4D81-9AD0-392D3273C6C2}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
-    <x:sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <x:sheet name="System Exceptions" sheetId="6" r:id="rId6"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="191029"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16395C6-4BAB-44F9-8C76-33F1BE7DB26B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{E61F36DB-E3C1-4D81-9AD0-392D3273C6C2}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="System Exceptions" sheetId="6" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <x:si>
-    <x:t>The Conclusion Evidence Location path: \\MainFolder\Remediation_or_Justification Evidence\1-09-2020\CHR0000928476.pdf for the change: CHANGES - SOX Audit Report for testps9023.txt_07.01.73.eml made on 1/9/2020 is not a valid path.</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,64 +385,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{0E39E9EB-0823-4512-9F06-C076B0D8756A}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:1">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E39E9EB-0823-4512-9F06-C076B0D8756A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{76068DCB-BAB5-434F-8014-2A099B63434F}" mc:Ignorable="x14ac xr xr2 xr3">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <x:sheetData/>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76068DCB-BAB5-434F-8014-2A099B63434F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1"/>
-  <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData/>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding some changes (but not really)
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -1,92 +1,127 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16395C6-4BAB-44F9-8C76-33F1BE7DB26B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{E61F36DB-E3C1-4D81-9AD0-392D3273C6C2}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="System Exceptions" sheetId="6" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B326E750-D8FE-4DB1-BF07-11C397EFA19D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="0" activeTab="0" xr2:uid="{E61F36DB-E3C1-4D81-9AD0-392D3273C6C2}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <x:sheet name="System Exceptions" sheetId="6" r:id="rId3"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    </x:ext>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <x:si>
+    <x:t>CHANGES - SOX...eml on date01/09/2020 00:00:00 is missing ITRCA Member that filed or reviewed final evidence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHANGES - SOX...eml on date01/13/2020 00:00:00 is missing ITRCA Member that filed or reviewed final evidence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHANGES - SOX...eml on date01/14/2020 00:00:00 is missing ITRCA Member that filed or reviewed final evidence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHANGES - SOX...eml on date01/22/2020 00:00:00 is missing ITRCA Member that filed or reviewed final evidence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CHANGES - SOX...eml on date01/24/2020 00:00:00 is missing ITRCA Member that filed or reviewed final evidence</x:t>
+  </x:si>
+  <x:si>
+    <x:t>{row.item(3).ToString + " " + row.item(0).ToString.Substring(0,10) +  " does not contain Server Name " + row.item(7).ToString}</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,41 +420,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E39E9EB-0823-4512-9F06-C076B0D8756A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{0E39E9EB-0823-4512-9F06-C076B0D8756A}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A2:A22"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="F5" sqref="F5 F5:F5 A1:XFD1048576"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <x:sheetData>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A2" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A3" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A4" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A5" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A6" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A7" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A8" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A9" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A10" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A11" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A12" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A13" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A14" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A15" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A16" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A17" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A18" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A19" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A20" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A21" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <x:c r="A22" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76068DCB-BAB5-434F-8014-2A099B63434F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{76068DCB-BAB5-434F-8014-2A099B63434F}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:A3"/>
+  <x:sheetViews>
+    <x:sheetView topLeftCell="A2" workbookViewId="0">
+      <x:selection activeCell="E2" sqref="E2 E2:E2 A1:XFD1048576"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <x:row r="2" spans="1:5" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <x:row r="3" spans="1:5" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
fixed printing to pdf error
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dylan\Documents\UiPath\Robotic_Process_Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B326E750-D8FE-4DB1-BF07-11C397EFA19D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0513620-AFAA-4E87-BA25-F5A4F19DE0BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="0" activeTab="0" xr2:uid="{E61F36DB-E3C1-4D81-9AD0-392D3273C6C2}"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="0" activeTab="0" xr2:uid="{325A0D12-9FD8-47D1-BCAC-4A91C2A5175E}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
@@ -102,8 +102,9 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -420,124 +421,315 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{0E39E9EB-0823-4512-9F06-C076B0D8756A}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{36A60BA7-0529-4D26-B31E-849C26A3C4E3}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A2:A22"/>
+  <x:dimension ref="A2:A62"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="F5" sqref="F5 F5:F5 A1:XFD1048576"/>
-    </x:sheetView>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:sheetData>
-    <x:row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A2" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A3" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A4" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A5" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A6" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A7" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A8" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A9" s="1" t="s">
+    <x:row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A6" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A7" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A8" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A9" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A10" s="1" t="s">
+    <x:row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A10" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A11" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A12" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A13" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A14" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A15" s="1" t="s">
+    <x:row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A11" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A12" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A13" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A14" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A15" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A16" s="1" t="s">
+    <x:row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A16" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A17" s="1" t="s">
+    <x:row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A17" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A18" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A19" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A20" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A21" s="2" t="s"/>
+    </x:row>
+    <x:row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A22" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A23" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A24" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A25" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A26" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A27" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A28" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A29" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A30" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A31" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A32" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A33" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A34" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A35" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A18" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A19" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A20" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A21" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <x:c r="A22" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:6"/>
+    <x:row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A36" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A37" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A38" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A39" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A40" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A41" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A43" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A44" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A45" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A46" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A47" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A48" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A49" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A50" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A51" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A52" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A53" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A54" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A55" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A56" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A57" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A58" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A59" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A60" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A61" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A62" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:1"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -548,7 +740,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{76068DCB-BAB5-434F-8014-2A099B63434F}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{8DD2BE38-3F65-448B-9455-9719376D4518}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -556,7 +748,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:sheetData/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -571,21 +763,15 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A3"/>
+  <x:dimension ref="A1"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="A2" workbookViewId="0">
-      <x:selection activeCell="E2" sqref="E2 E2:E2 A1:XFD1048576"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:5" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <x:row r="2" spans="1:5" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <x:row r="3" spans="1:5" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-  </x:sheetData>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetData/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>

<commit_message>
files will be overwritten
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0513620-AFAA-4E87-BA25-F5A4F19DE0BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA28754-61AC-4A2C-9B74-7C578F9C15C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="0" activeTab="0" xr2:uid="{325A0D12-9FD8-47D1-BCAC-4A91C2A5175E}"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="0" activeTab="0" xr2:uid="{AD127604-E5F9-4811-8B39-840820810D8A}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <x:sheet name="System Exceptions" sheetId="6" r:id="rId3"/>
+    <x:sheet name="System Exceptions" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191029"/>
@@ -102,9 +102,8 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -421,315 +420,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{36A60BA7-0529-4D26-B31E-849C26A3C4E3}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{94134A0C-E3B5-4A0C-AA78-17BF0DE01E86}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A2:A62"/>
+  <x:dimension ref="A2:A22"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:sheetData>
     <x:row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="2" t="s">
+      <x:c r="A2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A3" s="2" t="s">
+      <x:c r="A3" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="2" t="s">
+      <x:c r="A4" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="2" t="s">
+      <x:c r="A5" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A6" s="2" t="s">
+      <x:c r="A6" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A7" s="2" t="s">
+      <x:c r="A7" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A8" s="2" t="s">
+      <x:c r="A8" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A9" s="2" t="s">
+      <x:c r="A9" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A10" s="2" t="s">
+      <x:c r="A10" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A11" s="2" t="s">
+      <x:c r="A11" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A12" s="2" t="s">
+      <x:c r="A12" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A13" s="2" t="s">
+      <x:c r="A13" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A14" s="2" t="s">
+      <x:c r="A14" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A15" s="2" t="s">
+      <x:c r="A15" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A16" s="2" t="s">
+      <x:c r="A16" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A17" s="2" t="s">
+      <x:c r="A17" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A18" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A18" s="2" t="s">
+    <x:row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A19" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A19" s="2" t="s">
+    <x:row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A20" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A20" s="2" t="s">
+    <x:row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <x:c r="A21" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A21" s="2" t="s"/>
-    </x:row>
     <x:row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A22" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A23" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A24" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A25" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A26" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A27" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A28" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A29" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A30" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A31" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A32" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A33" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A34" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A35" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A36" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A37" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A38" s="2" t="s">
+      <x:c r="A22" s="1" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A39" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A40" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A41" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A43" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A44" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A45" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A46" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A47" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A48" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A49" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A50" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A51" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A52" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A53" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A54" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A55" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A56" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A57" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A58" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A59" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A60" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A61" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A62" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="63" spans="1:1"/>
+    <x:row r="23" spans="1:1"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -740,7 +546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{8DD2BE38-3F65-448B-9455-9719376D4518}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{206083C2-2E31-48F0-892F-C5BFC36EC0B3}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -759,7 +565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -767,7 +573,7 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
only have to output the section 3review sign off
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A596B110-041C-4C46-8D7F-1E2C5C717583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F221D74A-1563-4847-97B2-DEAF88FCC756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{C5D605D0-3E49-4D8D-8148-446A1529E164}"/>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="0" activeTab="0" xr2:uid="{7115F4FF-24B6-4644-8968-8CED01078169}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <x:sheet name="System Exceptions" sheetId="6" r:id="rId3"/>
+    <x:sheet name="System Exceptions" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <x:si>
     <x:t>CHANGES - SOX...eml does not have valid Reference Type in column I</x:t>
   </x:si>
@@ -44,6 +44,9 @@
     <x:t>CHANGES - SOX...eml on date01/09/2020 00:00:00 is missing ITRCA Member that filed or reviewed final evidence</x:t>
   </x:si>
   <x:si>
+    <x:t>CHANGES - SOX...eml on 01/24/2020 00:00:00 missing Server Name magic_kl02 (Expected Server Name)</x:t>
+  </x:si>
+  <x:si>
     <x:t>CHANGES - SOX Audit Report for magic_kl02.txt_07.01.73.eml01/13/2020does not contain Server Name magic_kq_023</x:t>
   </x:si>
   <x:si>
@@ -54,44 +57,6 @@
   </x:si>
   <x:si>
     <x:t>The Conclusion Evidence Location path: FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RE Random Email missing.msg for the change: CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml made on 1/22/2020 is not a valid path.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>System.IO.IOException: The process cannot access the file 'C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\outputExcel.xlsx' because it is being used by another process.
-   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)
-   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)
-   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share, Int32 bufferSize, FileOptions options, String msgPath, Boolean bFromProxy)
-   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share, Int32 bufferSize, Boolean useAsync)
-   at MS.Internal.IO.Zip.ZipArchive.OpenOnFile(String path, FileMode mode, FileAccess access, FileShare share, Boolean streaming)
-   at System.IO.Packaging.ZipPackage..ctor(String path, FileMode mode, FileAccess access, FileShare share, Boolean streaming)
-   at System.IO.Packaging.Package.Open(String path, FileMode packageMode, FileAccess packageAccess, FileShare packageShare, Boolean streaming)
-   at DocumentFormat.OpenXml.Packaging.OpenXmlPackage.OpenCore(String path, Boolean readWriteMode)
-   at DocumentFormat.OpenXml.Packaging.SpreadsheetDocument.Open(String path, Boolean isEditable, OpenSettings openSettings)
-   at ClosedXML.Excel.XLWorkbook.LoadSheets(String fileName) in C:\Projects\ClosedXML\ClosedXML\Excel\XLWorkbook_Load.cs:line 44
-   at UiPath.Excel.WorkbookFile..ctor(String workbookPath, String password, Boolean createNew)
-   at UiPath.Excel.Activities.WorkbookActivity`1.ConstructWorkbook(String path, String password, Boolean createNew)
-   at UiPath.Excel.Activities.WorkbookActivity`1.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)
-   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)
-   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)
-   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>System.IO.IOException: The process cannot access the file 'C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\outputExcel.xlsx' because it is being used by another process.
-   at System.IO.__Error.WinIOError(Int32 errorCode, String maybeFullPath)
-   at System.IO.FileStream.Init(String path, FileMode mode, FileAccess access, Int32 rights, Boolean useRights, FileShare share, Int32 bufferSize, FileOptions options, SECURITY_ATTRIBUTES secAttrs, String msgPath, Boolean bFromProxy, Boolean useLongPath, Boolean checkHost)
-   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share, Int32 bufferSize, FileOptions options, String msgPath, Boolean bFromProxy)
-   at System.IO.FileStream..ctor(String path, FileMode mode, FileAccess access, FileShare share, Int32 bufferSize, Boolean useAsync)
-   at MS.Internal.IO.Zip.ZipArchive.OpenOnFile(String path, FileMode mode, FileAccess access, FileShare share, Boolean streaming)
-   at System.IO.Packaging.ZipPackage..ctor(String path, FileMode mode, FileAccess access, FileShare share, Boolean streaming)
-   at System.IO.Packaging.Package.Open(String path, FileMode packageMode, FileAccess packageAccess, FileShare packageShare, Boolean streaming)
-   at DocumentFormat.OpenXml.Packaging.OpenXmlPackage.OpenCore(String path, Boolean readWriteMode)
-   at DocumentFormat.OpenXml.Packaging.SpreadsheetDocument.Open(String path, Boolean isEditable, OpenSettings openSettings)
-   at ClosedXML.Excel.XLWorkbook.LoadSheets(String fileName) in C:\Projects\ClosedXML\ClosedXML\Excel\XLWorkbook_Load.cs:line 44
-   at UiPath.Excel.WorkbookFile..ctor(String workbookPath, String password, Boolean createNew)
-   at UiPath.Excel.Activities.WorkbookActivity`1.ConstructWorkbook(String path, String password, Boolean createNew)
-   at UiPath.Excel.Activities.WorkbookActivity`1.BeginExecute(AsyncCodeActivityContext context, AsyncCallback callback, Object state)
-   at System.Activities.AsyncCodeActivity.InternalExecute(ActivityInstance instance, ActivityExecutor executor, BookmarkManager bookmarkManager)
-   at System.Activities.ActivityInstance.Execute(ActivityExecutor executor, BookmarkManager bookmarkManager)
-   at System.Activities.Runtime.ActivityExecutor.ExecuteActivityWorkItem.ExecuteBody(ActivityExecutor executor, BookmarkManager bookmarkManager, Location resultLocation)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -134,30 +99,16 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="5">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -472,92 +423,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{F59A8C0C-BE12-4AA5-8677-8431732C3304}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{2E725FB5-352C-4178-883F-F954BBBB2E6A}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A2:A16"/>
+  <x:dimension ref="A2:A9"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:sheetData>
     <x:row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="2" t="s">
+      <x:c r="A2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A3" s="2" t="s">
+      <x:c r="A3" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="2" t="s">
+      <x:c r="A4" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="2" t="s">
+      <x:c r="A5" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A6" s="2" t="s">
-        <x:v>2</x:v>
+      <x:c r="A6" s="1" t="s">
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A7" s="2" t="s">
+      <x:c r="A7" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A8" s="2" t="s">
+      <x:c r="A8" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A9" s="2" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A10" s="2" t="s">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A11" s="2" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A12" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A13" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A14" s="2" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A15" s="2" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A16" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:1">
-      <x:c r="A17" s="2" t="s">
+      <x:c r="A9" s="1" t="s">
         <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:1">
+      <x:c r="A10" s="1" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -570,7 +488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{2064E03E-1FDA-4D56-AE7B-0204674F24A9}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{6AA2F67A-5BA8-405C-A3BE-0B836D100606}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -589,7 +507,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -597,19 +515,8 @@
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:1">
-      <x:c r="A1" s="3" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:1">
-      <x:c r="A2" s="3" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData/>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>

<commit_message>
was able to populate database with exceptions
</commit_message>
<xml_diff>
--- a/Exceptions.xlsx
+++ b/Exceptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E7FBB3-277A-4571-99BE-536CC67A4C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE84912-352B-4117-BC00-0ABC8D8081C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="3696" yWindow="1680" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{5A7B1AED-DA37-492B-8CA9-87292AD1CF2B}"/>
+    <x:workbookView xWindow="3696" yWindow="1680" windowWidth="17280" windowHeight="8964" firstSheet="0" activeTab="0" xr2:uid="{A3DA47BC-D186-4137-9BB7-88011E82A8AB}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Business Exceptions" sheetId="2" r:id="rId1"/>
@@ -47,13 +47,13 @@
     <x:t>CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73.eml01/13/2020does not contain Server Name magic_kl02</x:t>
   </x:si>
   <x:si>
+    <x:t>The Conclusion Evidence Location path: FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\ for the change: CHANGES - SOX Audit Report for testps0324.txt_07.01.73.eml made on 1/9/2020 is not a valid path.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Conclusion Evidence Location path: FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\ for the change: CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml made on 1/22/2020 is not a valid path.</x:t>
+  </x:si>
+  <x:si>
     <x:t>The Conclusion Evidence Location path: FOLDER\Mainfolder\Remediation_or_Justification Evidence\Invalid Folder\1-14-2020\CHR0000291924.pdf for the change: CHANGES - SOX Audit Report for magic9843.txt_07.01.73.eml made on 1/14/2020 is not a valid path.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Conclusion Evidence Location path: FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-09-2020\RandomFolder1\ for the change: CHANGES - SOX Audit Report for testps0324.txt_07.01.73.eml made on 1/9/2020 is not a valid path.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Conclusion Evidence Location path: FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RandomFolder2\ for the change: CHANGES - SOX Audit Report for magic435.txt_07.01.73.eml made on 1/22/2020 is not a valid path.</x:t>
   </x:si>
   <x:si>
     <x:t>The Conclusion Evidence Location path: FOLDER\Mainfolder\Remediation_or_Justification Evidence\1-22-2020\RE Random Email missing.msg for the change: CHANGES - SOX Audit Report for test234234.txt_07.01.73.eml made on 1/22/2020 is not a valid path.</x:t>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00A642ED-0EAD-40F4-979A-169B5505DC60}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{8C16D382-69A2-4E63-B6D6-DA4348507F28}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{CD5C51C4-43B8-47BF-9674-4901E853D361}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{43FB5ABA-69E3-4D1F-980D-C0E54F42E6BE}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>

</xml_diff>